<commit_message>
Add time stamps and compute distance.  Remove call to start rotate.
</commit_message>
<xml_diff>
--- a/2017CompetitionBot/docs/RobotGearDeliverySchedule.xlsx
+++ b/2017CompetitionBot/docs/RobotGearDeliverySchedule.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dimentions of Field" sheetId="1" r:id="rId1"/>
@@ -382,26 +382,6 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
@@ -430,6 +410,26 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
@@ -490,20 +490,20 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A5:Q20" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A5:Q20" totalsRowShown="0" headerRowDxfId="9">
   <autoFilter ref="A5:Q20"/>
   <tableColumns count="17">
     <tableColumn id="1" name="# of gears"/>
-    <tableColumn id="2" name="Travel Distance (m)" dataDxfId="10">
+    <tableColumn id="2" name="Travel Distance (m)" dataDxfId="8">
       <calculatedColumnFormula>B5+15.5*2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" name="Travel Distance - Incl. overhead (m)" dataDxfId="9">
+    <tableColumn id="3" name="Travel Distance - Incl. overhead (m)" dataDxfId="7">
       <calculatedColumnFormula>B6*(1+Assumptions!$B$5)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Minimum speed required (m/s)" dataDxfId="8">
+    <tableColumn id="4" name="Minimum speed required (m/s)" dataDxfId="6">
       <calculatedColumnFormula>IF(K6&gt;0,C6/K6,"n/a")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Minimum Speed (km/hr)" dataDxfId="7">
+    <tableColumn id="5" name="Minimum Speed (km/hr)" dataDxfId="5">
       <calculatedColumnFormula>D6*60*60/1000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" name="Time spent Unloading the balls (s)">
@@ -522,19 +522,19 @@
     <tableColumn id="11" name="Travel Time (s)">
       <calculatedColumnFormula>Assumptions!$B$4-SUM(F6:J6)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" name="Seconds per Gears (s)" dataDxfId="6">
+    <tableColumn id="12" name="Seconds per Gears (s)" dataDxfId="4">
       <calculatedColumnFormula>IF(K6&gt;0,Assumptions!$B$4/A6,"n/a")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" name="Balls  Shot" dataDxfId="5">
+    <tableColumn id="14" name="Balls  Shot" dataDxfId="3">
       <calculatedColumnFormula>Assumptions!$B$13</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" name="Balls Successful" dataDxfId="4">
+    <tableColumn id="15" name="Balls Successful" dataDxfId="2">
       <calculatedColumnFormula>M6*Assumptions!$B$15</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" name="Points Per Ball" dataDxfId="3">
+    <tableColumn id="16" name="Points Per Ball" dataDxfId="1">
       <calculatedColumnFormula>1/3</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" name="Preasure Points Accumulated" dataDxfId="2">
+    <tableColumn id="17" name="Preasure Points Accumulated" dataDxfId="0">
       <calculatedColumnFormula>N6*O6</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" name="Comments"/>
@@ -1253,8 +1253,8 @@
   </sheetPr>
   <dimension ref="A3:D15"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1388,7 +1388,7 @@
         <v>45</v>
       </c>
       <c r="B13">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
         <v>46</v>
@@ -1435,7 +1435,7 @@
   </sheetPr>
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -1630,11 +1630,11 @@
       </c>
       <c r="M7" s="3">
         <f>M6+Assumptions!$B$13</f>
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="N7" s="3">
         <f>M7*Assumptions!$B$15</f>
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="O7" s="3">
         <f t="shared" ref="O7:O20" si="3">1/3</f>
@@ -1642,7 +1642,7 @@
       </c>
       <c r="P7" s="3">
         <f>P6+(N7-N6)*O7</f>
-        <v>9.3333333333333321</v>
+        <v>7.333333333333333</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.3">
@@ -1694,11 +1694,11 @@
       </c>
       <c r="M8" s="3">
         <f>M7+Assumptions!$B$13</f>
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="N8" s="3">
         <f>M8*Assumptions!$B$15</f>
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="O8" s="3">
         <f t="shared" si="3"/>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="P8" s="3">
         <f t="shared" ref="P8:P20" si="4">P7+(N8-N7)*O8</f>
-        <v>14.666666666666664</v>
+        <v>10.666666666666666</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.3">
@@ -1758,11 +1758,11 @@
       </c>
       <c r="M9" s="3">
         <f>M8+Assumptions!$B$13</f>
-        <v>130</v>
+        <v>85</v>
       </c>
       <c r="N9" s="3">
         <f>M9*Assumptions!$B$15</f>
-        <v>52</v>
+        <v>34</v>
       </c>
       <c r="O9" s="3">
         <f t="shared" si="3"/>
@@ -1770,7 +1770,7 @@
       </c>
       <c r="P9" s="3">
         <f t="shared" si="4"/>
-        <v>19.999999999999996</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.3">
@@ -1822,11 +1822,11 @@
       </c>
       <c r="M10" s="3">
         <f>M9+Assumptions!$B$13</f>
-        <v>170</v>
+        <v>110</v>
       </c>
       <c r="N10" s="3">
         <f>M10*Assumptions!$B$15</f>
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="O10" s="3">
         <f t="shared" si="3"/>
@@ -1834,7 +1834,7 @@
       </c>
       <c r="P10" s="3">
         <f t="shared" si="4"/>
-        <v>25.333333333333329</v>
+        <v>17.333333333333332</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -1886,11 +1886,11 @@
       </c>
       <c r="M11" s="3">
         <f>M10+Assumptions!$B$13</f>
-        <v>210</v>
+        <v>135</v>
       </c>
       <c r="N11" s="3">
         <f>M11*Assumptions!$B$15</f>
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="O11" s="3">
         <f t="shared" si="3"/>
@@ -1898,7 +1898,7 @@
       </c>
       <c r="P11" s="3">
         <f t="shared" si="4"/>
-        <v>30.666666666666661</v>
+        <v>20.666666666666664</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.3">
@@ -1950,11 +1950,11 @@
       </c>
       <c r="M12" s="3">
         <f>M11+Assumptions!$B$13</f>
-        <v>250</v>
+        <v>160</v>
       </c>
       <c r="N12" s="3">
         <f>M12*Assumptions!$B$15</f>
-        <v>100</v>
+        <v>64</v>
       </c>
       <c r="O12" s="3">
         <f t="shared" si="3"/>
@@ -1962,7 +1962,7 @@
       </c>
       <c r="P12" s="3">
         <f t="shared" si="4"/>
-        <v>35.999999999999993</v>
+        <v>23.999999999999996</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -2014,11 +2014,11 @@
       </c>
       <c r="M13" s="3">
         <f>M12+Assumptions!$B$13</f>
-        <v>290</v>
+        <v>185</v>
       </c>
       <c r="N13" s="3">
         <f>M13*Assumptions!$B$15</f>
-        <v>116</v>
+        <v>74</v>
       </c>
       <c r="O13" s="3">
         <f t="shared" si="3"/>
@@ -2026,7 +2026,7 @@
       </c>
       <c r="P13" s="3">
         <f t="shared" si="4"/>
-        <v>41.333333333333329</v>
+        <v>27.333333333333329</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.3">
@@ -2078,11 +2078,11 @@
       </c>
       <c r="M14" s="3">
         <f>M13+Assumptions!$B$13</f>
-        <v>330</v>
+        <v>210</v>
       </c>
       <c r="N14" s="3">
         <f>M14*Assumptions!$B$15</f>
-        <v>132</v>
+        <v>84</v>
       </c>
       <c r="O14" s="3">
         <f t="shared" si="3"/>
@@ -2090,7 +2090,7 @@
       </c>
       <c r="P14" s="3">
         <f t="shared" si="4"/>
-        <v>46.666666666666664</v>
+        <v>30.666666666666661</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.3">
@@ -2142,11 +2142,11 @@
       </c>
       <c r="M15" s="3">
         <f>M14+Assumptions!$B$13</f>
-        <v>370</v>
+        <v>235</v>
       </c>
       <c r="N15" s="3">
         <f>M15*Assumptions!$B$15</f>
-        <v>148</v>
+        <v>94</v>
       </c>
       <c r="O15" s="3">
         <f t="shared" si="3"/>
@@ -2154,7 +2154,7 @@
       </c>
       <c r="P15" s="3">
         <f t="shared" si="4"/>
-        <v>52</v>
+        <v>33.999999999999993</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.3">
@@ -2206,11 +2206,11 @@
       </c>
       <c r="M16" s="3">
         <f>M15+Assumptions!$B$13</f>
-        <v>410</v>
+        <v>260</v>
       </c>
       <c r="N16" s="3">
         <f>M16*Assumptions!$B$15</f>
-        <v>164</v>
+        <v>104</v>
       </c>
       <c r="O16" s="3">
         <f t="shared" si="3"/>
@@ -2218,7 +2218,7 @@
       </c>
       <c r="P16" s="3">
         <f t="shared" si="4"/>
-        <v>57.333333333333336</v>
+        <v>37.333333333333329</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.3">
@@ -2270,11 +2270,11 @@
       </c>
       <c r="M17" s="3">
         <f>M16+Assumptions!$B$13</f>
-        <v>450</v>
+        <v>285</v>
       </c>
       <c r="N17" s="3">
         <f>M17*Assumptions!$B$15</f>
-        <v>180</v>
+        <v>114</v>
       </c>
       <c r="O17" s="3">
         <f t="shared" si="3"/>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="P17" s="3">
         <f t="shared" si="4"/>
-        <v>62.666666666666671</v>
+        <v>40.666666666666664</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -2334,11 +2334,11 @@
       </c>
       <c r="M18" s="3">
         <f>M17+Assumptions!$B$13</f>
-        <v>490</v>
+        <v>310</v>
       </c>
       <c r="N18" s="3">
         <f>M18*Assumptions!$B$15</f>
-        <v>196</v>
+        <v>124</v>
       </c>
       <c r="O18" s="3">
         <f t="shared" si="3"/>
@@ -2346,7 +2346,7 @@
       </c>
       <c r="P18" s="3">
         <f t="shared" si="4"/>
-        <v>68</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
@@ -2398,11 +2398,11 @@
       </c>
       <c r="M19" s="3">
         <f>M18+Assumptions!$B$13</f>
-        <v>530</v>
+        <v>335</v>
       </c>
       <c r="N19" s="3">
         <f>M19*Assumptions!$B$15</f>
-        <v>212</v>
+        <v>134</v>
       </c>
       <c r="O19" s="3">
         <f t="shared" si="3"/>
@@ -2410,7 +2410,7 @@
       </c>
       <c r="P19" s="3">
         <f t="shared" si="4"/>
-        <v>73.333333333333329</v>
+        <v>47.333333333333336</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
@@ -2462,11 +2462,11 @@
       </c>
       <c r="M20" s="3">
         <f>M19+Assumptions!$B$13</f>
-        <v>570</v>
+        <v>360</v>
       </c>
       <c r="N20" s="3">
         <f>M20*Assumptions!$B$15</f>
-        <v>228</v>
+        <v>144</v>
       </c>
       <c r="O20" s="3">
         <f t="shared" si="3"/>
@@ -2474,7 +2474,7 @@
       </c>
       <c r="P20" s="3">
         <f t="shared" si="4"/>
-        <v>78.666666666666657</v>
+        <v>50.666666666666671</v>
       </c>
     </row>
   </sheetData>

</xml_diff>